<commit_message>
Issue#30  Req 5.5  fix 7.3 - run happy path and make sure file is created
</commit_message>
<xml_diff>
--- a/happyPathTest/SAP_04122018.xlsx
+++ b/happyPathTest/SAP_04122018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\devman-generator\findFilesTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\devman-generator\happyPathTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>First name</t>
   </si>
@@ -48,39 +48,21 @@
     <t>Staff</t>
   </si>
   <si>
-    <t>Corporate Services</t>
-  </si>
-  <si>
     <t>L3 (Expert)</t>
   </si>
   <si>
     <t>601505</t>
   </si>
   <si>
-    <t>Project Governance</t>
-  </si>
-  <si>
     <t>Delivery</t>
   </si>
   <si>
-    <t>600928</t>
-  </si>
-  <si>
     <t>L4 (Professional)</t>
   </si>
   <si>
     <t>L7 (Leader)</t>
   </si>
   <si>
-    <t>Business Development</t>
-  </si>
-  <si>
-    <t>Business Consulting</t>
-  </si>
-  <si>
-    <t>Gr IT Service Mgmt</t>
-  </si>
-  <si>
     <t>Pers.no. Mentor</t>
   </si>
   <si>
@@ -96,40 +78,34 @@
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>Tomasz</t>
-  </si>
-  <si>
-    <t>Jurek</t>
-  </si>
-  <si>
     <t>TZJE</t>
   </si>
   <si>
-    <t xml:space="preserve">Dariusz </t>
-  </si>
-  <si>
-    <t>Szymon</t>
-  </si>
-  <si>
-    <t>Kaczmarczyk</t>
-  </si>
-  <si>
     <t>DZLI</t>
   </si>
   <si>
     <t>SNKK</t>
   </si>
   <si>
-    <t>Łęcki</t>
-  </si>
-  <si>
     <t>Personnel Subarea</t>
   </si>
   <si>
-    <t>Warsaw</t>
-  </si>
-  <si>
     <t>Lodz</t>
+  </si>
+  <si>
+    <t>Mentee</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>BestMentor</t>
+  </si>
+  <si>
+    <t>Project Development</t>
   </si>
 </sst>
 </file>
@@ -978,7 +954,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1008,10 +984,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1026,139 +1002,139 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D2" s="4">
-        <v>600334</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I2" s="5">
         <v>41764</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
       </c>
       <c r="L2" s="7">
         <v>30582</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="4">
-        <v>600125</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I3" s="5">
-        <v>39295</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>13</v>
+        <v>41764</v>
+      </c>
+      <c r="J3" s="4">
+        <v>123</v>
       </c>
       <c r="K3" s="4">
-        <v>600334</v>
+        <v>456</v>
       </c>
       <c r="L3" s="7">
         <v>33443</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4">
-        <v>666655</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I4" s="5">
-        <v>37854</v>
+        <v>41764</v>
       </c>
       <c r="J4" s="4">
-        <v>600334</v>
+        <v>456</v>
       </c>
       <c r="K4" s="4">
-        <v>600334</v>
+        <v>123</v>
       </c>
       <c r="L4" s="7">
         <v>29426</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue#30  Req 5.5  fix public class PreferDevManThatIsOlderThan30YearsOldStrategy VotingStrategy  fix Test 1.16 Mentor above 30 years old and older is  preferred for Mentee  change  .filter(sympathyResultTuple -> sympathyResultTuple.sympathy != SympathyResult. None)  to  .filter(sympathyResultTuple -> !SympathyResult.None.equals(sympathyResultTuple.sympathy))  as comparing should be done by equals instead of reference
</commit_message>
<xml_diff>
--- a/happyPathTest/SAP_04122018.xlsx
+++ b/happyPathTest/SAP_04122018.xlsx
@@ -954,7 +954,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G5" sqref="G5:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1034,7 +1034,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>10</v>
@@ -1075,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>10</v>
@@ -1090,7 +1090,7 @@
         <v>456</v>
       </c>
       <c r="L3" s="7">
-        <v>33443</v>
+        <v>31982</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Issue#30  Req 5.5  happy path -> writing to file line by line with candidates proposed
</commit_message>
<xml_diff>
--- a/happyPathTest/SAP_04122018.xlsx
+++ b/happyPathTest/SAP_04122018.xlsx
@@ -954,7 +954,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1087,7 +1087,7 @@
         <v>123</v>
       </c>
       <c r="K3" s="4">
-        <v>456</v>
+        <v>789</v>
       </c>
       <c r="L3" s="7">
         <v>31982</v>
@@ -1128,7 +1128,7 @@
         <v>456</v>
       </c>
       <c r="K4" s="4">
-        <v>123</v>
+        <v>91011</v>
       </c>
       <c r="L4" s="7">
         <v>29426</v>

</xml_diff>